<commit_message>
Update variabels_table.xlsx with new data
</commit_message>
<xml_diff>
--- a/data/variabels_table.xlsx
+++ b/data/variabels_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhakbarhamid21/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhakbarhamid21/Pelatihan/IDCamp 2024/Kelas Mahir/Submission/Submission Akhir - Menyelesaikan Permasalahan Institusi Pendidikan/student-dropout-prediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121AA736-9974-C84B-A84E-0214E36FB71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E24726D-DFBF-A843-A2D0-8E16E56CB069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="21000" xr2:uid="{B62D02AB-0854-D74E-A440-7E6920F924CB}"/>
+    <workbookView xWindow="5160" yWindow="22100" windowWidth="33600" windowHeight="19240" xr2:uid="{B62D02AB-0854-D74E-A440-7E6920F924CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7668B121-B506-FF41-B448-6BA94C46F2CA}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>